<commit_message>
2021/2/15 mac を commit
</commit_message>
<xml_diff>
--- a/Program/出荷実績照会_土気.xlsx
+++ b/Program/出荷実績照会_土気.xlsx
@@ -8,10 +8,10 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="新潟運輸_通常_輸出N" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ケイヒン_通常_輸出Y" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="西濃_通常_輸出N" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="トール_通常_輸出N" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ケイヒン_通常_輸出N" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ケイヒン_通常_輸出N" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="トール_通常_輸出N" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ケイヒン_通常_輸出Y" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="西濃_通常_輸出N" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
@@ -783,6 +783,822 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="2.42" customWidth="1" min="1" max="1"/>
+    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
+    <col width="8.030000000000001" customWidth="1" min="3" max="3"/>
+    <col width="30.69" customWidth="1" min="4" max="4"/>
+    <col width="10.45" customWidth="1" min="5" max="5"/>
+    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
+    <col width="4.29" customWidth="1" min="7" max="7"/>
+    <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
+    <col width="4.29" customWidth="1" min="9" max="9"/>
+    <col width="7.15" customWidth="1" min="10" max="10"/>
+    <col width="1.65" customWidth="1" min="11" max="11"/>
+    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="23" customHeight="1">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>出荷実績照会</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>出荷工場：@0002 土気工場</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>運送業者：U0007 ケイヒン   配送区分：1 通常  輸出：N</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>行</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>売上日</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>納入先名</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>品名</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>ﾛｯﾄNo.</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>売上数量</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>単位</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>注文No.</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>缶数</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>備考</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>ＡＳ－５ＮＰ艶消アンダー (15KG)</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>21010802H</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr"/>
+      <c r="I5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr"/>
+      <c r="L5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>ＡＳ－５ＮＰ艶消アンダー (15KG)</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>21020805H</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr"/>
+      <c r="I6" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr"/>
+      <c r="L6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>ＵＬ－１００リターダー (15KG)</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>20111306H</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr"/>
+      <c r="I7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr"/>
+      <c r="L7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>ＫＳ－０４２　Ｂ液　（１５ＫＧ）</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>21020303H</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H8" s="1" t="inlineStr"/>
+      <c r="I8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K8" s="1" t="inlineStr"/>
+      <c r="L8" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>ＫＳ－０４２　Ａ液　（１５ＫＧ）</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>21020210H</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H9" s="1" t="inlineStr"/>
+      <c r="I9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="J9" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K9" s="1" t="inlineStr"/>
+      <c r="L9" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>ＡタイプＰＰ反射板用塗料 (15KG)</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>21020405H</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H10" s="1" t="inlineStr"/>
+      <c r="I10" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="J10" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K10" s="1" t="inlineStr"/>
+      <c r="L10" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="18" customHeight="1">
+      <c r="A11" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>ＡＳ－５ＮＰクリヤー (15KG)</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr">
+        <is>
+          <t>20112604H</t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H11" s="1" t="inlineStr"/>
+      <c r="I11" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="J11" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K11" s="1" t="inlineStr"/>
+      <c r="L11" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="18" customHeight="1">
+      <c r="A12" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>Ｕ－３３０ シンナー (14KG)</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>20111910H</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H12" s="1" t="inlineStr"/>
+      <c r="I12" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K12" s="1" t="inlineStr"/>
+      <c r="L12" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="18" customHeight="1">
+      <c r="A13" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>Ｕ－３３０ シンナー (14KG)</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>21011903H</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H13" s="1" t="inlineStr"/>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K13" s="1" t="inlineStr"/>
+      <c r="L13" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="2.42" customWidth="1" min="1" max="1"/>
+    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
+    <col width="8.030000000000001" customWidth="1" min="3" max="3"/>
+    <col width="21.34" customWidth="1" min="4" max="4"/>
+    <col width="10.45" customWidth="1" min="5" max="5"/>
+    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
+    <col width="4.29" customWidth="1" min="7" max="7"/>
+    <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
+    <col width="4.29" customWidth="1" min="9" max="9"/>
+    <col width="32.34" customWidth="1" min="10" max="10"/>
+    <col width="1.65" customWidth="1" min="11" max="11"/>
+    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="23" customHeight="1">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>出荷実績照会</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>出荷工場：@0002 土気工場</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>運送業者：U0001 トール   配送区分：1 通常  輸出：N</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>行</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>売上日</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>納入先名</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>品名</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>ﾛｯﾄNo.</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>売上数量</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>単位</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>注文No.</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>缶数</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>備考</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>ＹＫＰ</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>ＭＢ－２０Ｋ２ (15KG)</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>21011352T</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr"/>
+      <c r="I5" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr"/>
+      <c r="L5" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v/>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>ADM-1（1KG)</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr"/>
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr"/>
+      <c r="I6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>表面処理事業部　事業部長　三枝様宛</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr"/>
+      <c r="L6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v/>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>UHU-5315B（1KG)</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr"/>
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr"/>
+      <c r="I7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>表面処理事業部　事業部長　三枝様宛</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr"/>
+      <c r="L7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>20210215</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v/>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>UHU-5315A（1KG)</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr"/>
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H8" s="1" t="inlineStr"/>
+      <c r="I8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="inlineStr">
+        <is>
+          <t>表面処理事業部　事業部長　三枝様宛</t>
+        </is>
+      </c>
+      <c r="K8" s="1" t="inlineStr"/>
+      <c r="L8" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1111,7 +1927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1279,822 +2095,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:L8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="2.42" customWidth="1" min="1" max="1"/>
-    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
-    <col width="8.030000000000001" customWidth="1" min="3" max="3"/>
-    <col width="21.34" customWidth="1" min="4" max="4"/>
-    <col width="10.45" customWidth="1" min="5" max="5"/>
-    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
-    <col width="4.29" customWidth="1" min="7" max="7"/>
-    <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
-    <col width="4.29" customWidth="1" min="9" max="9"/>
-    <col width="32.34" customWidth="1" min="10" max="10"/>
-    <col width="1.65" customWidth="1" min="11" max="11"/>
-    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="23" customHeight="1">
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>出荷実績照会</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="18" customHeight="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>出荷工場：@0002 土気工場</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18" customHeight="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>運送業者：U0001 トール   配送区分：1 通常  輸出：N</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18" customHeight="1">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>行</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>売上日</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>納入先名</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>品名</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>ﾛｯﾄNo.</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>売上数量</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>単位</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>注文No.</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>缶数</t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t>備考</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="L4" s="1" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="18" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>ＹＫＰ</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>ＭＢ－２０Ｋ２ (15KG)</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>21011352T</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr"/>
-      <c r="I5" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr"/>
-      <c r="L5" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" ht="18" customHeight="1">
-      <c r="A6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v/>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>ADM-1（1KG)</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr"/>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr"/>
-      <c r="I6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>表面処理事業部　事業部長　三枝様宛</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr"/>
-      <c r="L6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v/>
-      </c>
-      <c r="D7" s="1" t="inlineStr">
-        <is>
-          <t>UHU-5315B（1KG)</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="inlineStr"/>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H7" s="1" t="inlineStr"/>
-      <c r="I7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>表面処理事業部　事業部長　三枝様宛</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr"/>
-      <c r="L7" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="18" customHeight="1">
-      <c r="A8" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v/>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>UHU-5315A（1KG)</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr"/>
-      <c r="F8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H8" s="1" t="inlineStr"/>
-      <c r="I8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>表面処理事業部　事業部長　三枝様宛</t>
-        </is>
-      </c>
-      <c r="K8" s="1" t="inlineStr"/>
-      <c r="L8" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:L13"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="2.42" customWidth="1" min="1" max="1"/>
-    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
-    <col width="8.030000000000001" customWidth="1" min="3" max="3"/>
-    <col width="30.69" customWidth="1" min="4" max="4"/>
-    <col width="10.45" customWidth="1" min="5" max="5"/>
-    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
-    <col width="4.29" customWidth="1" min="7" max="7"/>
-    <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
-    <col width="4.29" customWidth="1" min="9" max="9"/>
-    <col width="7.15" customWidth="1" min="10" max="10"/>
-    <col width="1.65" customWidth="1" min="11" max="11"/>
-    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="23" customHeight="1">
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>出荷実績照会</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="18" customHeight="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>出荷工場：@0002 土気工場</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18" customHeight="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>運送業者：U0007 ケイヒン   配送区分：1 通常  輸出：N</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18" customHeight="1">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>行</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>売上日</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>納入先名</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>品名</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>ﾛｯﾄNo.</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>売上数量</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>単位</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>注文No.</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>缶数</t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t>備考</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="L4" s="1" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="18" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>ＡＳ－５ＮＰ艶消アンダー (15KG)</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>21010802H</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr"/>
-      <c r="I5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr"/>
-      <c r="L5" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="18" customHeight="1">
-      <c r="A6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>ＡＳ－５ＮＰ艶消アンダー (15KG)</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>21020805H</t>
-        </is>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr"/>
-      <c r="I6" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr"/>
-      <c r="L6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="inlineStr">
-        <is>
-          <t>ＵＬ－１００リターダー (15KG)</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>20111306H</t>
-        </is>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H7" s="1" t="inlineStr"/>
-      <c r="I7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr"/>
-      <c r="L7" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="18" customHeight="1">
-      <c r="A8" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>ＫＳ－０４２　Ｂ液　（１５ＫＧ）</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>21020303H</t>
-        </is>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H8" s="1" t="inlineStr"/>
-      <c r="I8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K8" s="1" t="inlineStr"/>
-      <c r="L8" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" ht="18" customHeight="1">
-      <c r="A9" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>ＫＳ－０４２　Ａ液　（１５ＫＧ）</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>21020210H</t>
-        </is>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H9" s="1" t="inlineStr"/>
-      <c r="I9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K9" s="1" t="inlineStr"/>
-      <c r="L9" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" ht="18" customHeight="1">
-      <c r="A10" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="inlineStr">
-        <is>
-          <t>ＡタイプＰＰ反射板用塗料 (15KG)</t>
-        </is>
-      </c>
-      <c r="E10" s="1" t="inlineStr">
-        <is>
-          <t>21020405H</t>
-        </is>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H10" s="1" t="inlineStr"/>
-      <c r="I10" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="J10" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K10" s="1" t="inlineStr"/>
-      <c r="L10" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" ht="18" customHeight="1">
-      <c r="A11" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D11" s="1" t="inlineStr">
-        <is>
-          <t>ＡＳ－５ＮＰクリヤー (15KG)</t>
-        </is>
-      </c>
-      <c r="E11" s="1" t="inlineStr">
-        <is>
-          <t>20112604H</t>
-        </is>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H11" s="1" t="inlineStr"/>
-      <c r="I11" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="J11" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K11" s="1" t="inlineStr"/>
-      <c r="L11" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" ht="18" customHeight="1">
-      <c r="A12" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D12" s="1" t="inlineStr">
-        <is>
-          <t>Ｕ－３３０ シンナー (14KG)</t>
-        </is>
-      </c>
-      <c r="E12" s="1" t="inlineStr">
-        <is>
-          <t>20111910H</t>
-        </is>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G12" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H12" s="1" t="inlineStr"/>
-      <c r="I12" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="J12" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K12" s="1" t="inlineStr"/>
-      <c r="L12" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" ht="18" customHeight="1">
-      <c r="A13" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>20210215</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t>伊坂藤枝</t>
-        </is>
-      </c>
-      <c r="D13" s="1" t="inlineStr">
-        <is>
-          <t>Ｕ－３３０ シンナー (14KG)</t>
-        </is>
-      </c>
-      <c r="E13" s="1" t="inlineStr">
-        <is>
-          <t>21011903H</t>
-        </is>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H13" s="1" t="inlineStr"/>
-      <c r="I13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K13" s="1" t="inlineStr"/>
-      <c r="L13" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
20210218 管理単位にBI を追加 packing.py
</commit_message>
<xml_diff>
--- a/Program/出荷実績照会_土気.xlsx
+++ b/Program/出荷実績照会_土気.xlsx
@@ -7,11 +7,14 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="西濃_通常_輸出N" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="トール_通常_輸出N" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="ケイヒン_通常_輸出N" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="NoData_通常_輸出N" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ケイヒン_通常_輸出N" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="トール_通常_輸出N" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="新潟運輸_通常_輸出N" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sheet" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="西濃_通常_輸出N" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="トール_通常_輸出Y" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ケイヒン_通常_輸出Y" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Sheet" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -238,6 +241,96 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2400300" cy="595312"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2400300" cy="595312"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2400300" cy="595312"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -566,14 +659,14 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="2.42"/>
     <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
-    <col customWidth="1" max="3" min="3" width="8.030000000000001"/>
-    <col customWidth="1" max="4" min="4" width="32.23"/>
+    <col customWidth="1" max="3" min="3" width="19.25"/>
+    <col customWidth="1" max="4" min="4" width="33.55"/>
     <col customWidth="1" max="5" min="5" width="10.45"/>
     <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
     <col customWidth="1" max="7" min="7" width="4.29"/>
-    <col customWidth="1" max="8" min="8" width="9.350000000000001"/>
+    <col customWidth="1" max="8" min="8" width="8.25"/>
     <col customWidth="1" max="9" min="9" width="4.29"/>
-    <col customWidth="1" max="10" min="10" width="19.58"/>
+    <col customWidth="1" max="10" min="10" width="7.15"/>
     <col customWidth="1" max="11" min="11" width="1.65"/>
     <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
   </cols>
@@ -595,7 +688,7 @@
     <row customHeight="1" ht="18" r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>運送業者：U0003 西濃   配送区分：1 通常  輸出：N</t>
+          <t>運送業者：NoData NoData   配送区分：1 通常  輸出：N</t>
         </is>
       </c>
     </row>
@@ -667,41 +760,43 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>西鉄　成田梱包営業所</t>
+        </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>ＳＶ－３８００ＬＨＲアンダー(1KG)</t>
+          <t>ＳＴＭ-３０-Ｔ１ メタル (UN/25KG)</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>21010751T</t>
+          <t>21021603H</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>CN</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
-          <t>Q9019935</t>
+          <t>FG10099</t>
         </is>
       </c>
       <c r="I5" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>工場72受入担当：楠様</t>
+          <t>noData</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr"/>
@@ -717,6 +812,472 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="2.42"/>
+    <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
+    <col customWidth="1" max="3" min="3" width="8.030000000000001"/>
+    <col customWidth="1" max="4" min="4" width="26.95"/>
+    <col customWidth="1" max="5" min="5" width="10.45"/>
+    <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
+    <col customWidth="1" max="7" min="7" width="4.29"/>
+    <col customWidth="1" max="8" min="8" width="7.590000000000001"/>
+    <col customWidth="1" max="9" min="9" width="4.29"/>
+    <col customWidth="1" max="10" min="10" width="8.690000000000001"/>
+    <col customWidth="1" max="11" min="11" width="1.65"/>
+    <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="23" r="1">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>出荷実績照会</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>出荷工場：@0002 土気工場</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>運送業者：U0007 ケイヒン   配送区分：1 通常  輸出：N</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>行</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>売上日</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>納入先名</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>品名</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>ﾛｯﾄNo.</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>売上数量</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>単位</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>注文No.</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>缶数</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>備考</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="5">
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>ＲＴ－４８トップ (14KG)</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>21012952T</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr"/>
+      <c r="I5" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr"/>
+      <c r="L5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="6">
+      <c r="A6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>ＵＶ－３０５アンダー (15KG)</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>21021551T</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr"/>
+      <c r="I6" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>2/22納期</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr"/>
+      <c r="L6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="7">
+      <c r="A7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>伊坂藤枝</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>ＲＴ－４５ トップ (14KG)</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>20120153T</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr"/>
+      <c r="I7" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr"/>
+      <c r="L7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.8" footer="0.5" header="0.5" left="0.2" right="0.2" top="0.8"/>
+  <pageSetup fitToHeight="0" fitToWidth="1" orientation="landscape" paperSize="9"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="2.42"/>
+    <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
+    <col customWidth="1" max="3" min="3" width="9.9"/>
+    <col customWidth="1" max="4" min="4" width="25.08"/>
+    <col customWidth="1" max="5" min="5" width="10.45"/>
+    <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
+    <col customWidth="1" max="7" min="7" width="4.29"/>
+    <col customWidth="1" max="8" min="8" width="7.590000000000001"/>
+    <col customWidth="1" max="9" min="9" width="4.29"/>
+    <col customWidth="1" max="10" min="10" width="18.04"/>
+    <col customWidth="1" max="11" min="11" width="1.65"/>
+    <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="23" r="1">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>出荷実績照会</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>出荷工場：@0002 土気工場</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>運送業者：U0001 トール   配送区分：1 通常  輸出：N</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>行</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>売上日</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>納入先名</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>品名</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>ﾛｯﾄNo.</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>売上数量</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>単位</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>注文No.</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>缶数</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>備考</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="5">
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>光輝社焼津</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>ＫＶ－３８アンダー (15KG)</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>21011853T</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr"/>
+      <c r="I5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>2/22納期　土気出荷</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr"/>
+      <c r="L5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="6">
+      <c r="A6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>東海化成</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>ＭＢ－２０Ｋ２ (15KG)</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>21011352T</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr"/>
+      <c r="I6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>2/24納期</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr"/>
+      <c r="L6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.8" footer="0.5" header="0.5" left="0.2" right="0.2" top="0.8"/>
+  <pageSetup fitToHeight="0" fitToWidth="1" orientation="landscape" paperSize="9"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -732,14 +1293,14 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="2.75"/>
     <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
-    <col customWidth="1" max="3" min="3" width="8.030000000000001"/>
-    <col customWidth="1" max="4" min="4" width="32.56"/>
+    <col customWidth="1" max="3" min="3" width="13.64"/>
+    <col customWidth="1" max="4" min="4" width="33.77"/>
     <col customWidth="1" max="5" min="5" width="10.45"/>
     <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
     <col customWidth="1" max="7" min="7" width="4.29"/>
-    <col customWidth="1" max="8" min="8" width="7.590000000000001"/>
+    <col customWidth="1" max="8" min="8" width="11.55"/>
     <col customWidth="1" max="9" min="9" width="4.29"/>
-    <col customWidth="1" max="10" min="10" width="7.15"/>
+    <col customWidth="1" max="10" min="10" width="31.02"/>
     <col customWidth="1" max="11" min="11" width="1.65"/>
     <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
   </cols>
@@ -761,7 +1322,7 @@
     <row customHeight="1" ht="18" r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>運送業者：U0001 トール   配送区分：1 通常  輸出：N</t>
+          <t>運送業者：U0009 新潟運輸   配送区分：1 通常  輸出：N</t>
         </is>
       </c>
     </row>
@@ -833,41 +1394,35 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>柏真空</t>
+        </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Ｘ－８０ＮＰアンダー(15KG)</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>21010631H</t>
-        </is>
-      </c>
+          <t>染料液レッドLQ（0.1KG）</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>NO.3</t>
-        </is>
-      </c>
+          <t>BI</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr"/>
       <c r="I5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
+          <t>石井社長宛</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr"/>
@@ -881,37 +1436,31 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>相模塗装</t>
+        </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>ＢＰ－５０アンダー (15KG)</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>21012951T</t>
-        </is>
-      </c>
+          <t>ＢＳ－４２１ Ｂ液 (4KG)</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>NO.3</t>
-        </is>
-      </c>
+      <c r="H6" s="1" t="inlineStr"/>
       <c r="I6" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
@@ -920,7 +1469,7 @@
       </c>
       <c r="K6" s="1" t="inlineStr"/>
       <c r="L6" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="7">
@@ -929,37 +1478,31 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>相模塗装</t>
+        </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>ＢＳ－４２１ Ａ液 (15KG)</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>20120952T</t>
-        </is>
-      </c>
+          <t>ＢＳ－４２１Ａ－ＢＬＫ (4KG)</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="H7" s="1" t="inlineStr">
-        <is>
-          <t>NO.3</t>
-        </is>
-      </c>
+      <c r="H7" s="1" t="inlineStr"/>
       <c r="I7" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
@@ -968,7 +1511,7 @@
       </c>
       <c r="K7" s="1" t="inlineStr"/>
       <c r="L7" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="8">
@@ -977,41 +1520,39 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>スタンレー秦野</t>
+        </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>ＢＳ－４２１ Ｂ液 (15KG)</t>
+          <t>ＳＶ－３８００アンダー　（1KG）</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>20110502H</t>
+          <t>20111251T</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H8" s="1" t="inlineStr">
-        <is>
-          <t>NO.3</t>
-        </is>
-      </c>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="H8" s="1" t="inlineStr"/>
       <c r="I8" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
+          <t>2/22納期　土気出荷　一号館NO.80</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr"/>
@@ -1025,37 +1566,39 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>スタンレー岡崎</t>
+        </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>ＰＰ－４４ＮＰアンダー (15KG)</t>
+          <t>ＳＶ－３８００Ｌ　アンダー　（1KG）</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>20072801H</t>
+          <t>21011251T</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>KG</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
         <is>
-          <t>NO.3</t>
+          <t>K7112342</t>
         </is>
       </c>
       <c r="I9" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
@@ -1073,41 +1616,43 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>南部化成　裾野</t>
+        </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>ＲＴ－３５Ｍ トップ (16KG)</t>
+          <t>ＵＶ－５４２アンダー　（1KG）</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>21011902H</t>
+          <t>21011452T</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>KG</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>NO.3</t>
+          <t>2101221016</t>
         </is>
       </c>
       <c r="I10" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J10" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
+          <t>2/22納期 根上様</t>
         </is>
       </c>
       <c r="K10" s="1" t="inlineStr"/>
@@ -1121,37 +1666,43 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>南部化成　裾野</t>
+        </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>ＵＶ－５４２ アンダー (15KG)</t>
+          <t>ＲＴ－１６０ＨＮＶトップ　（1KG）</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>21011452T</t>
+          <t>20091851T</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H11" s="1" t="inlineStr"/>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="H11" s="1" t="inlineStr">
+        <is>
+          <t>2101221039</t>
+        </is>
+      </c>
       <c r="I11" s="1" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J11" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
+          <t>2/22納期 根上様</t>
         </is>
       </c>
       <c r="K11" s="1" t="inlineStr"/>
@@ -1165,37 +1716,43 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>南部化成　裾野</t>
+        </is>
       </c>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>ＳＴ－３２金色Ｔ－５ (15KG)</t>
+          <t>Ａ－８２０　シンナー　(1KG)</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>20101950T</t>
+          <t>20112702H</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H12" s="1" t="inlineStr"/>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="H12" s="1" t="inlineStr">
+        <is>
+          <t>2101221019</t>
+        </is>
+      </c>
       <c r="I12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J12" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
+          <t>2/22納期 根上様</t>
         </is>
       </c>
       <c r="K12" s="1" t="inlineStr"/>
@@ -1209,37 +1766,43 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>南部化成　裾野</t>
+        </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>ＳＴ－３２金色Ｔ－５ (15KG)</t>
+          <t>Ａ－８２０　シンナー　(1KG)</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>21010750T</t>
+          <t>21012001H</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H13" s="1" t="inlineStr"/>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="H13" s="1" t="inlineStr">
+        <is>
+          <t>2101221019</t>
+        </is>
+      </c>
       <c r="I13" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J13" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
+          <t>2/22納期 根上様</t>
         </is>
       </c>
       <c r="K13" s="1" t="inlineStr"/>
@@ -1253,24 +1816,26 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>市光工業伊勢原</t>
+        </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>ＳＴ－３２金色　Ｃ－３０９ (15KG)</t>
+          <t>ＢＳ－４２１Ａ－ＢＬＫ (4KG)</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>21021750T</t>
+          <t>21020152T</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1" t="inlineStr">
         <is>
@@ -1279,11 +1844,11 @@
       </c>
       <c r="H14" s="1" t="inlineStr"/>
       <c r="I14" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
+          <t>2/22納期</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr"/>
@@ -1298,13 +1863,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1314,12 +1879,230 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="2.42"/>
     <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
-    <col customWidth="1" max="3" min="3" width="8.030000000000001"/>
-    <col customWidth="1" max="4" min="4" width="34.09999999999999"/>
+    <col customWidth="1" max="3" min="3" width="13.64"/>
+    <col customWidth="1" max="4" min="4" width="32.23"/>
     <col customWidth="1" max="5" min="5" width="10.45"/>
     <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
     <col customWidth="1" max="7" min="7" width="4.29"/>
-    <col customWidth="1" max="8" min="8" width="7.590000000000001"/>
+    <col customWidth="1" max="8" min="8" width="9.350000000000001"/>
+    <col customWidth="1" max="9" min="9" width="4.29"/>
+    <col customWidth="1" max="10" min="10" width="19.58"/>
+    <col customWidth="1" max="11" min="11" width="1.65"/>
+    <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="23" r="1">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>出荷実績照会</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>出荷工場：@0002 土気工場</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>運送業者：U0003 西濃   配送区分：1 通常  輸出：N</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>行</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>売上日</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>納入先名</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>品名</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>ﾛｯﾄNo.</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>売上数量</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>単位</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>注文No.</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>缶数</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>備考</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="5">
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>スタンレー浜松</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>ＳＶ－３８００ＬＨＲアンダー(1KG)</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>21010751T</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>Q9021409</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>工場72受入担当：楠様</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr"/>
+      <c r="L5" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="6">
+      <c r="A6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>スタンレー浜松</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>ＳＶ－３８００ＬＨＲアンダー(1KG)</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>21010751T</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>Q9021263</t>
+        </is>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>工場72受入担当：楠様</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr"/>
+      <c r="L6" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.8" footer="0.5" header="0.5" left="0.2" right="0.2" top="0.8"/>
+  <pageSetup fitToHeight="0" fitToWidth="1" orientation="landscape" paperSize="9"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="2.42"/>
+    <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
+    <col customWidth="1" max="3" min="3" width="13.64"/>
+    <col customWidth="1" max="4" min="4" width="33.55"/>
+    <col customWidth="1" max="5" min="5" width="10.45"/>
+    <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
+    <col customWidth="1" max="7" min="7" width="4.29"/>
+    <col customWidth="1" max="8" min="8" width="12.65"/>
     <col customWidth="1" max="9" min="9" width="4.29"/>
     <col customWidth="1" max="10" min="10" width="8.690000000000001"/>
     <col customWidth="1" max="11" min="11" width="1.65"/>
@@ -1343,7 +2126,7 @@
     <row customHeight="1" ht="18" r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>運送業者：U0007 ケイヒン   配送区分：1 通常  輸出：N</t>
+          <t>運送業者：U0001 トール   配送区分：1 通常  輸出：Y</t>
         </is>
       </c>
     </row>
@@ -1415,40 +2198,50 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>日本通運　成田</t>
+        </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Ｎ－４０４（改２）アンダー (15KG)</t>
+          <t>Ｋ－７０６ＣＬ(改) Ｂ液 (UN/17KG)</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>21020501H</t>
+          <t>21020904H</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="H5" s="1" t="inlineStr"/>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>HEC-INK20K2</t>
+        </is>
+      </c>
       <c r="I5" s="1" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>2/19納期</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr"/>
+          <t>2/22納期</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
       <c r="L5" s="1" t="n">
         <v>1</v>
       </c>
@@ -1459,40 +2252,50 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>西鉄物流</t>
+        </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Ｂタイプ反射板用塗料 (4KG)</t>
+          <t>ＰＰ反射板用Ｂタイプ (UN/15KG)</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>21020903H</t>
+          <t>21020901H</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="H6" s="1" t="inlineStr"/>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>TTW2691</t>
+        </is>
+      </c>
       <c r="I6" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
           <t>noData</t>
         </is>
       </c>
-      <c r="K6" s="1" t="inlineStr"/>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
       <c r="L6" s="1" t="n">
         <v>1</v>
       </c>
@@ -1503,169 +2306,51 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>西鉄物流</t>
+        </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>ＢタイプＰＰ反射板用塗料 (15KG)</t>
+          <t>ＰＰ反射板用Ｃタイプ (UN/15KG)</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>21020902H</t>
+          <t>21021101H</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="H7" s="1" t="inlineStr"/>
+      <c r="H7" s="1" t="inlineStr">
+        <is>
+          <t>TTW2691</t>
+        </is>
+      </c>
       <c r="I7" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
           <t>noData</t>
         </is>
       </c>
-      <c r="K7" s="1" t="inlineStr"/>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
       <c r="L7" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="18" r="8">
-      <c r="A8" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v/>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>ＰＲ－Ａ・Ｓ　希釈用シンナー (４KG)</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>21021510H</t>
-        </is>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H8" s="1" t="inlineStr"/>
-      <c r="I8" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K8" s="1" t="inlineStr"/>
-      <c r="L8" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="18" r="9">
-      <c r="A9" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v/>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>P-5プライマー　(1KG)</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr"/>
-      <c r="F9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H9" s="1" t="inlineStr"/>
-      <c r="I9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K9" s="1" t="inlineStr"/>
-      <c r="L9" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="18" r="10">
-      <c r="A10" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v/>
-      </c>
-      <c r="D10" s="1" t="inlineStr">
-        <is>
-          <t>ＲＴＳ－０４アンダー (15KG)</t>
-        </is>
-      </c>
-      <c r="E10" s="1" t="inlineStr">
-        <is>
-          <t>21012651T</t>
-        </is>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="G10" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H10" s="1" t="inlineStr"/>
-      <c r="I10" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="J10" s="1" t="inlineStr">
-        <is>
-          <t>2/19納期</t>
-        </is>
-      </c>
-      <c r="K10" s="1" t="inlineStr"/>
-      <c r="L10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1676,7 +2361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1692,14 +2377,14 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="2.42"/>
     <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
-    <col customWidth="1" max="3" min="3" width="14.3"/>
-    <col customWidth="1" max="4" min="4" width="28.16"/>
+    <col customWidth="1" max="3" min="3" width="12.87"/>
+    <col customWidth="1" max="4" min="4" width="27.61"/>
     <col customWidth="1" max="5" min="5" width="10.45"/>
     <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
     <col customWidth="1" max="7" min="7" width="4.29"/>
-    <col customWidth="1" max="8" min="8" width="11.55"/>
+    <col customWidth="1" max="8" min="8" width="8.25"/>
     <col customWidth="1" max="9" min="9" width="4.29"/>
-    <col customWidth="1" max="10" min="10" width="15.4"/>
+    <col customWidth="1" max="10" min="10" width="8.690000000000001"/>
     <col customWidth="1" max="11" min="11" width="1.65"/>
     <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
   </cols>
@@ -1721,7 +2406,7 @@
     <row customHeight="1" ht="18" r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>運送業者：U0009 新潟運輸   配送区分：1 通常  輸出：N</t>
+          <t>運送業者：U0007 ケイヒン   配送区分：1 通常  輸出：Y</t>
         </is>
       </c>
     </row>
@@ -1793,40 +2478,46 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>名港海運西2区</t>
+        </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>ＫＶ－３８アンダー (15KG)</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>20121651T</t>
-        </is>
-      </c>
+          <t>ＰＴ－０４トップ (UN/15KG)</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="H5" s="1" t="inlineStr"/>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>TTL1220</t>
+        </is>
+      </c>
       <c r="I5" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr"/>
+          <t>2/22納期</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
       <c r="L5" s="1" t="n">
         <v>1</v>
       </c>
@@ -1837,40 +2528,50 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>名港海運西2区</t>
+        </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>ＫＶ－３８アンダー (15KG)</t>
+          <t>ＡＡＳ№１ Ａ液 (UN/15KG)</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>21011853T</t>
+          <t>21021002H</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="H6" s="1" t="inlineStr"/>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>TTL1220</t>
+        </is>
+      </c>
       <c r="I6" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr"/>
+          <t>2/22納期</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
       <c r="L6" s="1" t="n">
         <v>1</v>
       </c>
@@ -1881,46 +2582,50 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
+          <t>20210219</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>ｻｶｯｸ㈱本社工場</t>
+          <t>名港海運西2区</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Ａ－８２０　シンナー　(1KG)</t>
+          <t>ＡＡＳ№１ Ｂ液 (UN/15KG)</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>20112702H</t>
+          <t>21021102H</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>CN</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
-          <t>K7088255</t>
+          <t>TTL1220</t>
         </is>
       </c>
       <c r="I7" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr"/>
+          <t>2/22納期</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
       <c r="L7" s="1" t="n">
         <v>1</v>
       </c>
@@ -1931,44 +2636,50 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>20210218</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v/>
+          <t>20210219</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>名港海運西2区</t>
+        </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>ＵＶ－５４２アンダー　（1KG）</t>
+          <t>ＰＲ－Ａ（ＫＡI） (UN/15KG)</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>21011452T</t>
+          <t>21020213H</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>CN</t>
         </is>
       </c>
       <c r="H8" s="1" t="inlineStr">
         <is>
-          <t>2101221015</t>
+          <t>TTL1220</t>
         </is>
       </c>
       <c r="I8" s="1" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>2/19納期 根上様</t>
-        </is>
-      </c>
-      <c r="K8" s="1" t="inlineStr"/>
+          <t>2/22納期</t>
+        </is>
+      </c>
+      <c r="K8" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
       <c r="L8" s="1" t="n">
         <v>1</v>
       </c>
@@ -1980,7 +2691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
20210224 Downloaded untin_keisan_sheet from SQLserver
</commit_message>
<xml_diff>
--- a/Program/出荷実績照会_土気.xlsx
+++ b/Program/出荷実績照会_土気.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="新潟運輸_通常_輸出N" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="西濃_通常_輸出N" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="トール_通常_輸出Y" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="西濃_通常_輸出N" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="新潟運輸_通常_輸出N" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="トール_通常_輸出Y" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -65,16 +65,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>7</col>
@@ -158,17 +158,17 @@
     <ext cx="2400300" cy="595312"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>7</col>
@@ -188,17 +188,17 @@
     <ext cx="2400300" cy="595312"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>7</col>
@@ -218,17 +218,17 @@
     <ext cx="2400300" cy="595312"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -520,7 +520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
@@ -533,42 +533,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="2.42"/>
-    <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
-    <col customWidth="1" max="3" min="3" width="9.9"/>
-    <col customWidth="1" max="4" min="4" width="28.82"/>
-    <col customWidth="1" max="5" min="5" width="10.45"/>
-    <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
-    <col customWidth="1" max="7" min="7" width="4.29"/>
-    <col customWidth="1" max="8" min="8" width="7.590000000000001"/>
-    <col customWidth="1" max="9" min="9" width="4.29"/>
-    <col customWidth="1" max="10" min="10" width="8.690000000000001"/>
-    <col customWidth="1" max="11" min="11" width="1.65"/>
-    <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
+    <col width="2.42" customWidth="1" min="1" max="1"/>
+    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
+    <col width="14.63" customWidth="1" min="3" max="3"/>
+    <col width="32.23" customWidth="1" min="4" max="4"/>
+    <col width="10.45" customWidth="1" min="5" max="5"/>
+    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
+    <col width="4.29" customWidth="1" min="7" max="7"/>
+    <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
+    <col width="4.29" customWidth="1" min="9" max="9"/>
+    <col width="8.690000000000001" customWidth="1" min="10" max="10"/>
+    <col width="1.65" customWidth="1" min="11" max="11"/>
+    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="23" r="1">
+    <row r="1" ht="23" customHeight="1">
       <c r="E1" t="inlineStr">
         <is>
           <t>出荷実績照会</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="2">
+    <row r="2" ht="18" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
           <t>出荷工場：@0002 土気工場</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="3">
+    <row r="3" ht="18" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
-          <t>運送業者：U0009 新潟運輸   配送区分：1 通常  輸出：N</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="18" r="4">
+          <t>運送業者：U0003 西濃   配送区分：1 通常  輸出：N</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>行</t>
@@ -630,7 +630,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="5">
+    <row r="5" ht="18" customHeight="1">
       <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
@@ -641,30 +641,30 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>光輝社焼津</t>
+          <t>スタンレー浜松</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>ＵＶ－５４２ アンダー (15KG)</t>
+          <t>ＳＶ－３８００ＬＨＲアンダー(1KG)</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>21011452T</t>
+          <t>21010751T</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>KG</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr"/>
       <c r="I5" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
@@ -676,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="6">
+    <row r="6" ht="18" customHeight="1">
       <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
@@ -687,21 +687,21 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>新潟三桂</t>
+          <t>ﾌｧﾙﾃｯｸ　北関東</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Ｕ－１００ シンナー (15KG)</t>
+          <t>ＵＶ－２３００Ｌアンダー (15KG)</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>21011805H</t>
+          <t>21012552T</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
@@ -710,11 +710,11 @@
       </c>
       <c r="H6" s="1" t="inlineStr"/>
       <c r="I6" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>2/25納期</t>
+          <t>2/24納期</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr"/>
@@ -722,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="7">
+    <row r="7" ht="18" customHeight="1">
       <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
@@ -733,21 +733,21 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>新潟三桂</t>
+          <t>ﾌｧﾙﾃｯｸ　北関東</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>ＦＧ－３０００アンダー (15KG)</t>
+          <t>ＵＶ－２３００Ｌアンダー (15KG)</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>20120753T</t>
+          <t>21021251T</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
@@ -756,11 +756,11 @@
       </c>
       <c r="H7" s="1" t="inlineStr"/>
       <c r="I7" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>2/25納期</t>
+          <t>2/24納期</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr"/>
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="8">
+    <row r="8" ht="18" customHeight="1">
       <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
@@ -779,21 +779,21 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>新潟三桂</t>
+          <t>ﾌｧﾙﾃｯｸ　北関東</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>ＲＴ－４５ トップ (14KG)</t>
+          <t>ＵＶ－３８２Ｖトップ（１５ＫＧ）</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>20120153T</t>
+          <t>21012051T</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
@@ -802,11 +802,11 @@
       </c>
       <c r="H8" s="1" t="inlineStr"/>
       <c r="I8" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>2/25納期</t>
+          <t>2/24納期</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr"/>
@@ -814,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="9">
+    <row r="9" ht="18" customHeight="1">
       <c r="A9" s="1" t="n">
         <v>5</v>
       </c>
@@ -825,21 +825,21 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>新潟三桂</t>
+          <t>ﾌｧﾙﾃｯｸ　北関東</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>ＲＴ－４５ トップ (14KG)</t>
+          <t>ＵＶ－３８２Ｖトップ（１５ＫＧ）</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>21021652T</t>
+          <t>21021152T</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
@@ -848,11 +848,11 @@
       </c>
       <c r="H9" s="1" t="inlineStr"/>
       <c r="I9" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>2/25納期</t>
+          <t>2/24納期</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr"/>
@@ -861,14 +861,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.8" footer="0.5" header="0.5" left="0.2" right="0.2" top="0.8"/>
-  <pageSetup fitToHeight="0" fitToWidth="1" orientation="landscape" paperSize="9"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
@@ -881,42 +881,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="2.42"/>
-    <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
-    <col customWidth="1" max="3" min="3" width="14.63"/>
-    <col customWidth="1" max="4" min="4" width="32.23"/>
-    <col customWidth="1" max="5" min="5" width="10.45"/>
-    <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
-    <col customWidth="1" max="7" min="7" width="4.29"/>
-    <col customWidth="1" max="8" min="8" width="7.590000000000001"/>
-    <col customWidth="1" max="9" min="9" width="4.29"/>
-    <col customWidth="1" max="10" min="10" width="8.690000000000001"/>
-    <col customWidth="1" max="11" min="11" width="1.65"/>
-    <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
+    <col width="2.42" customWidth="1" min="1" max="1"/>
+    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
+    <col width="9.9" customWidth="1" min="3" max="3"/>
+    <col width="28.82" customWidth="1" min="4" max="4"/>
+    <col width="10.45" customWidth="1" min="5" max="5"/>
+    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
+    <col width="4.29" customWidth="1" min="7" max="7"/>
+    <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
+    <col width="4.29" customWidth="1" min="9" max="9"/>
+    <col width="8.690000000000001" customWidth="1" min="10" max="10"/>
+    <col width="1.65" customWidth="1" min="11" max="11"/>
+    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="23" r="1">
+    <row r="1" ht="23" customHeight="1">
       <c r="E1" t="inlineStr">
         <is>
           <t>出荷実績照会</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="2">
+    <row r="2" ht="18" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
           <t>出荷工場：@0002 土気工場</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="3">
+    <row r="3" ht="18" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
-          <t>運送業者：U0003 西濃   配送区分：1 通常  輸出：N</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="18" r="4">
+          <t>運送業者：U0009 新潟運輸   配送区分：1 通常  輸出：N</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>行</t>
@@ -978,7 +978,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="5">
+    <row r="5" ht="18" customHeight="1">
       <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
@@ -989,30 +989,30 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>スタンレー浜松</t>
+          <t>光輝社焼津</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>ＳＶ－３８００ＬＨＲアンダー(1KG)</t>
+          <t>ＵＶ－５４２ アンダー (15KG)</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>21010751T</t>
+          <t>21011452T</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>CN</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr"/>
       <c r="I5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
@@ -1024,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="6">
+    <row r="6" ht="18" customHeight="1">
       <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
@@ -1035,21 +1035,21 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>ﾌｧﾙﾃｯｸ　北関東</t>
+          <t>新潟三桂</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>ＵＶ－２３００Ｌアンダー (15KG)</t>
+          <t>ＲＴ－４５ トップ (14KG)</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>21012552T</t>
+          <t>20120153T</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
@@ -1058,11 +1058,11 @@
       </c>
       <c r="H6" s="1" t="inlineStr"/>
       <c r="I6" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>2/24納期</t>
+          <t>2/25納期</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr"/>
@@ -1070,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="7">
+    <row r="7" ht="18" customHeight="1">
       <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
@@ -1081,21 +1081,21 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>ﾌｧﾙﾃｯｸ　北関東</t>
+          <t>新潟三桂</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>ＵＶ－２３００Ｌアンダー (15KG)</t>
+          <t>ＲＴ－４５ トップ (14KG)</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>21021251T</t>
+          <t>21021652T</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
@@ -1104,11 +1104,11 @@
       </c>
       <c r="H7" s="1" t="inlineStr"/>
       <c r="I7" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>2/24納期</t>
+          <t>2/25納期</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr"/>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="8">
+    <row r="8" ht="18" customHeight="1">
       <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
@@ -1127,21 +1127,21 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>ﾌｧﾙﾃｯｸ　北関東</t>
+          <t>新潟三桂</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>ＵＶ－３８２Ｖトップ（１５ＫＧ）</t>
+          <t>Ｕ－１００ シンナー (15KG)</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>21012051T</t>
+          <t>21011805H</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
@@ -1150,11 +1150,11 @@
       </c>
       <c r="H8" s="1" t="inlineStr"/>
       <c r="I8" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>2/24納期</t>
+          <t>2/25納期</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr"/>
@@ -1162,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="9">
+    <row r="9" ht="18" customHeight="1">
       <c r="A9" s="1" t="n">
         <v>5</v>
       </c>
@@ -1173,21 +1173,21 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>ﾌｧﾙﾃｯｸ　北関東</t>
+          <t>新潟三桂</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>ＵＶ－３８２Ｖトップ（１５ＫＧ）</t>
+          <t>ＦＧ－３０００アンダー (15KG)</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>21021152T</t>
+          <t>20120753T</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
@@ -1196,11 +1196,11 @@
       </c>
       <c r="H9" s="1" t="inlineStr"/>
       <c r="I9" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>2/24納期</t>
+          <t>2/25納期</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr"/>
@@ -1209,14 +1209,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.8" footer="0.5" header="0.5" left="0.2" right="0.2" top="0.8"/>
-  <pageSetup fitToHeight="0" fitToWidth="1" orientation="landscape" paperSize="9"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1229,42 +1229,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="2.42"/>
-    <col customWidth="1" max="2" min="2" width="9.350000000000001"/>
-    <col customWidth="1" max="3" min="3" width="8.030000000000001"/>
-    <col customWidth="1" max="4" min="4" width="34.21"/>
-    <col customWidth="1" max="5" min="5" width="10.45"/>
-    <col customWidth="1" max="6" min="6" width="8.030000000000001"/>
-    <col customWidth="1" max="7" min="7" width="4.29"/>
-    <col customWidth="1" max="8" min="8" width="8.25"/>
-    <col customWidth="1" max="9" min="9" width="4.29"/>
-    <col customWidth="1" max="10" min="10" width="8.690000000000001"/>
-    <col customWidth="1" max="11" min="11" width="1.65"/>
-    <col customWidth="1" max="12" min="12" width="3.850000000000001"/>
+    <col width="2.42" customWidth="1" min="1" max="1"/>
+    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
+    <col width="8.030000000000001" customWidth="1" min="3" max="3"/>
+    <col width="34.21" customWidth="1" min="4" max="4"/>
+    <col width="10.45" customWidth="1" min="5" max="5"/>
+    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
+    <col width="4.29" customWidth="1" min="7" max="7"/>
+    <col width="8.25" customWidth="1" min="8" max="8"/>
+    <col width="4.29" customWidth="1" min="9" max="9"/>
+    <col width="8.690000000000001" customWidth="1" min="10" max="10"/>
+    <col width="1.65" customWidth="1" min="11" max="11"/>
+    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="23" r="1">
+    <row r="1" ht="23" customHeight="1">
       <c r="E1" t="inlineStr">
         <is>
           <t>出荷実績照会</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="2">
+    <row r="2" ht="18" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
           <t>出荷工場：@0002 土気工場</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="3">
+    <row r="3" ht="18" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
           <t>運送業者：U0001 トール   配送区分：1 通常  輸出：Y</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="4">
+    <row r="4" ht="18" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>行</t>
@@ -1326,7 +1326,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="5">
+    <row r="5" ht="18" customHeight="1">
       <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="6">
+    <row r="6" ht="18" customHeight="1">
       <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="7">
+    <row r="7" ht="18" customHeight="1">
       <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
@@ -1489,9 +1489,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.8" footer="0.5" header="0.5" left="0.2" right="0.2" top="0.8"/>
-  <pageSetup fitToHeight="0" fitToWidth="1" orientation="landscape" paperSize="9"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1509,6 +1509,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2021/2/26 JDT,untin_keisan_sheet,urigae_sumi をsqlserverから直接download UUの出荷予定倉庫を更新してからlogに表示するようにした
</commit_message>
<xml_diff>
--- a/Program/出荷実績照会_土気.xlsx
+++ b/Program/出荷実績照会_土気.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="西濃_通常_輸出N" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="新潟運輸_通常_輸出N" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="トール_通常_輸出Y" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="トール_曜日違い_輸出N" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
@@ -525,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,14 +535,14 @@
   <cols>
     <col width="2.42" customWidth="1" min="1" max="1"/>
     <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
-    <col width="14.63" customWidth="1" min="3" max="3"/>
+    <col width="13.64" customWidth="1" min="3" max="3"/>
     <col width="32.23" customWidth="1" min="4" max="4"/>
     <col width="10.45" customWidth="1" min="5" max="5"/>
     <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
     <col width="4.29" customWidth="1" min="7" max="7"/>
-    <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
+    <col width="9.350000000000001" customWidth="1" min="8" max="8"/>
     <col width="4.29" customWidth="1" min="9" max="9"/>
-    <col width="8.690000000000001" customWidth="1" min="10" max="10"/>
+    <col width="19.58" customWidth="1" min="10" max="10"/>
     <col width="1.65" customWidth="1" min="11" max="11"/>
     <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
   </cols>
@@ -636,7 +636,7 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>20210222</t>
+          <t>20210226</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -655,208 +655,28 @@
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
       </c>
-      <c r="H5" s="1" t="inlineStr"/>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>Q9037763</t>
+        </is>
+      </c>
       <c r="I5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>noData</t>
+          <t>工場72受入担当：楠様</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr"/>
       <c r="L5" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="18" customHeight="1">
-      <c r="A6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>20210222</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>ﾌｧﾙﾃｯｸ　北関東</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>ＵＶ－２３００Ｌアンダー (15KG)</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>21012552T</t>
-        </is>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr"/>
-      <c r="I6" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>2/24納期</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr"/>
-      <c r="L6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>20210222</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>ﾌｧﾙﾃｯｸ　北関東</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="inlineStr">
-        <is>
-          <t>ＵＶ－２３００Ｌアンダー (15KG)</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>21021251T</t>
-        </is>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H7" s="1" t="inlineStr"/>
-      <c r="I7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>2/24納期</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr"/>
-      <c r="L7" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="18" customHeight="1">
-      <c r="A8" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>20210222</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>ﾌｧﾙﾃｯｸ　北関東</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>ＵＶ－３８２Ｖトップ（１５ＫＧ）</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>21012051T</t>
-        </is>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H8" s="1" t="inlineStr"/>
-      <c r="I8" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>2/24納期</t>
-        </is>
-      </c>
-      <c r="K8" s="1" t="inlineStr"/>
-      <c r="L8" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" ht="18" customHeight="1">
-      <c r="A9" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>20210222</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>ﾌｧﾙﾃｯｸ　北関東</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>ＵＶ－３８２Ｖトップ（１５ＫＧ）</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>21021152T</t>
-        </is>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H9" s="1" t="inlineStr"/>
-      <c r="I9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t>2/24納期</t>
-        </is>
-      </c>
-      <c r="K9" s="1" t="inlineStr"/>
-      <c r="L9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -873,7 +693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -884,13 +704,13 @@
     <col width="2.42" customWidth="1" min="1" max="1"/>
     <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
     <col width="9.9" customWidth="1" min="3" max="3"/>
-    <col width="28.82" customWidth="1" min="4" max="4"/>
+    <col width="36.3" customWidth="1" min="4" max="4"/>
     <col width="10.45" customWidth="1" min="5" max="5"/>
     <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
     <col width="4.29" customWidth="1" min="7" max="7"/>
     <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
     <col width="4.29" customWidth="1" min="9" max="9"/>
-    <col width="8.690000000000001" customWidth="1" min="10" max="10"/>
+    <col width="7.15" customWidth="1" min="10" max="10"/>
     <col width="1.65" customWidth="1" min="11" max="11"/>
     <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
   </cols>
@@ -984,22 +804,22 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>20210222</t>
+          <t>20210226</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>光輝社焼津</t>
+          <t>海野技研</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>ＵＶ－５４２ アンダー (15KG)</t>
+          <t>ＳＴ－３２ＮＰＡ（改）銅色５５ (15KG)</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>21011452T</t>
+          <t>21022450T</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
@@ -1021,7 +841,7 @@
       </c>
       <c r="K5" s="1" t="inlineStr"/>
       <c r="L5" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" ht="18" customHeight="1">
@@ -1030,26 +850,26 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>20210222</t>
+          <t>20210226</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>新潟三桂</t>
+          <t>川口真空</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>ＲＴ－４５ トップ (14KG)</t>
+          <t>ＵＶ－２７０Ｍ アンダー（15kg）</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>20120153T</t>
+          <t>21011551T</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
@@ -1058,11 +878,11 @@
       </c>
       <c r="H6" s="1" t="inlineStr"/>
       <c r="I6" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>2/25納期</t>
+          <t>noData</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr"/>
@@ -1076,26 +896,26 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>20210222</t>
+          <t>20210226</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>新潟三桂</t>
+          <t>川口真空</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>ＲＴ－４５ トップ (14KG)</t>
+          <t>Ｕ－３３０ シンナー (14KG)</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>21021652T</t>
+          <t>21011903H</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
@@ -1104,11 +924,11 @@
       </c>
       <c r="H7" s="1" t="inlineStr"/>
       <c r="I7" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>2/25納期</t>
+          <t>noData</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr"/>
@@ -1122,26 +942,26 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>20210222</t>
+          <t>20210226</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>新潟三桂</t>
+          <t>光輝社焼津</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Ｕ－１００ シンナー (15KG)</t>
+          <t>ＫＶ－３８アンダー (15KG)</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>21011805H</t>
+          <t>21011853T</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
@@ -1150,11 +970,11 @@
       </c>
       <c r="H8" s="1" t="inlineStr"/>
       <c r="I8" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>2/25納期</t>
+          <t>noData</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr"/>
@@ -1168,26 +988,26 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>20210222</t>
+          <t>20210226</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>新潟三桂</t>
+          <t>光輝社焼津</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>ＦＧ－３０００アンダー (15KG)</t>
+          <t>ＵＶ－５４２ アンダー (15KG)</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>20120753T</t>
+          <t>21011452T</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
@@ -1196,15 +1016,61 @@
       </c>
       <c r="H9" s="1" t="inlineStr"/>
       <c r="I9" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>2/25納期</t>
+          <t>noData</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr"/>
       <c r="L9" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>20210226</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>三栄産業</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>ＦＰＡ－３(改)２アンダー (18㍑)</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>21011301H</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H10" s="1" t="inlineStr"/>
+      <c r="I10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1" t="inlineStr">
+        <is>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K10" s="1" t="inlineStr"/>
+      <c r="L10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1221,7 +1087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1232,13 +1098,13 @@
     <col width="2.42" customWidth="1" min="1" max="1"/>
     <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
     <col width="8.030000000000001" customWidth="1" min="3" max="3"/>
-    <col width="34.21" customWidth="1" min="4" max="4"/>
+    <col width="33.55" customWidth="1" min="4" max="4"/>
     <col width="10.45" customWidth="1" min="5" max="5"/>
     <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
     <col width="4.29" customWidth="1" min="7" max="7"/>
     <col width="8.25" customWidth="1" min="8" max="8"/>
     <col width="4.29" customWidth="1" min="9" max="9"/>
-    <col width="8.690000000000001" customWidth="1" min="10" max="10"/>
+    <col width="7.15" customWidth="1" min="10" max="10"/>
     <col width="1.65" customWidth="1" min="11" max="11"/>
     <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
   </cols>
@@ -1260,7 +1126,7 @@
     <row r="3" ht="18" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
-          <t>運送業者：U0001 トール   配送区分：1 通常  輸出：Y</t>
+          <t>運送業者：U0001 トール   配送区分：4 曜日違い  輸出：N</t>
         </is>
       </c>
     </row>
@@ -1332,22 +1198,20 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>20210222</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>日本通運</t>
-        </is>
+          <t>20210226</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v/>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Ｋ－７０６ＣＬ Ｂ液 (UN/17KG)</t>
+          <t>ＳＴＭ-３０-Ｔ１ メタル (UN/25KG)</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>21020905H</t>
+          <t>21020503H</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
@@ -1360,7 +1224,7 @@
       </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
-          <t>TTLG16</t>
+          <t>FG10092</t>
         </is>
       </c>
       <c r="I5" s="1" t="n">
@@ -1368,123 +1232,11 @@
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>2/24納期</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
+          <t>noData</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr"/>
       <c r="L5" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="18" customHeight="1">
-      <c r="A6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>20210222</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>日本通運</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>ＰＲ－Ｓ(改) Ａ液(ｸﾘﾔｰ）(UN/15KG)</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>21020803H</t>
-        </is>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>TTL1230</t>
-        </is>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>2/24納期</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>20210222</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>日本通運</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="inlineStr">
-        <is>
-          <t>ＰＲ－Ｓ(改) Ｂ液(ｱﾙﾐ）(UN/15KG)</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>21020804H</t>
-        </is>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H7" s="1" t="inlineStr">
-        <is>
-          <t>TTL1230</t>
-        </is>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>2/24納期</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="L7" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>